<commit_message>
created many methods for user interface @lumrachele
</commit_message>
<xml_diff>
--- a/bin/flights-app.xlsx
+++ b/bin/flights-app.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agamy/Development/module-one-final-project-guidelines-nyc-web-111918/bin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C7344204-A23B-0848-8B42-BDBBA8CD6289}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDBF9CC-C82A-B74F-A4AC-B1FB1417D1C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -868,7 +868,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1703,11 +1703,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D460"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="O365" workbookViewId="0">
+      <selection activeCell="B390" sqref="B390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>